<commit_message>
A4 - data & ranking
</commit_message>
<xml_diff>
--- a/Compsci361/A4/results.xlsx
+++ b/Compsci361/A4/results.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hasnaij\Desktop\University2020\Compsci361\A4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F7C121-B83F-495E-AD42-01EA0B49A20F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BF7A59-E0CE-4C79-AF48-7AAB31185634}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Accuracy" sheetId="1" r:id="rId1"/>
+    <sheet name="Ranking Matrix" sheetId="2" r:id="rId2"/>
+    <sheet name="Feature Ranking" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Simple Imputation Pre</t>
   </si>
@@ -44,12 +46,15 @@
   <si>
     <t>Average</t>
   </si>
+  <si>
+    <t>Top features</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,6 +74,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -106,12 +116,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,11 +429,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
@@ -428,7 +441,7 @@
     <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -442,7 +455,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -459,7 +472,7 @@
         <v>0.92024539877300615</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -476,7 +489,7 @@
         <v>0.93558282208588961</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -493,7 +506,7 @@
         <v>0.91717791411042948</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -510,7 +523,7 @@
         <v>0.89877300613496935</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -527,7 +540,7 @@
         <v>0.94478527607361962</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -544,7 +557,7 @@
         <v>0.8926380368098159</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -561,7 +574,7 @@
         <v>0.91104294478527603</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -578,7 +591,7 @@
         <v>0.93251533742331283</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -595,7 +608,7 @@
         <v>0.92638036809815949</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -612,7 +625,7 @@
         <v>0.90797546012269936</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -629,7 +642,7 @@
         <v>0.67576687116564416</v>
       </c>
       <c r="E13">
-        <f t="shared" ref="C13:E13" si="0">AVERAGE(E2:E11)</f>
+        <f t="shared" ref="E13" si="0">AVERAGE(E2:E11)</f>
         <v>0.91871165644171771</v>
       </c>
     </row>
@@ -637,4 +650,508 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B73A34DC-3F30-47C8-BFA4-A2B3F64E68E2}">
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>2669</v>
+      </c>
+      <c r="B2">
+        <v>2669</v>
+      </c>
+      <c r="C2">
+        <v>2669</v>
+      </c>
+      <c r="D2">
+        <v>699</v>
+      </c>
+      <c r="E2">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>309</v>
+      </c>
+      <c r="B3">
+        <v>719</v>
+      </c>
+      <c r="C3">
+        <v>699</v>
+      </c>
+      <c r="D3">
+        <v>3019</v>
+      </c>
+      <c r="E3">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>3048</v>
+      </c>
+      <c r="B4">
+        <v>699</v>
+      </c>
+      <c r="C4">
+        <v>2669</v>
+      </c>
+      <c r="D4">
+        <v>719</v>
+      </c>
+      <c r="E4">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>309</v>
+      </c>
+      <c r="B5">
+        <v>3019</v>
+      </c>
+      <c r="C5">
+        <v>2669</v>
+      </c>
+      <c r="D5">
+        <v>719</v>
+      </c>
+      <c r="E5">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>719</v>
+      </c>
+      <c r="B6">
+        <v>2669</v>
+      </c>
+      <c r="C6">
+        <v>3019</v>
+      </c>
+      <c r="D6">
+        <v>699</v>
+      </c>
+      <c r="E6">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>3048</v>
+      </c>
+      <c r="B7">
+        <v>699</v>
+      </c>
+      <c r="C7">
+        <v>2668</v>
+      </c>
+      <c r="D7">
+        <v>3019</v>
+      </c>
+      <c r="E7">
+        <v>3018</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>2669</v>
+      </c>
+      <c r="B8">
+        <v>719</v>
+      </c>
+      <c r="C8">
+        <v>309</v>
+      </c>
+      <c r="D8">
+        <v>699</v>
+      </c>
+      <c r="E8">
+        <v>3019</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>719</v>
+      </c>
+      <c r="B9">
+        <v>3049</v>
+      </c>
+      <c r="C9">
+        <v>2669</v>
+      </c>
+      <c r="D9">
+        <v>3019</v>
+      </c>
+      <c r="E9">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>309</v>
+      </c>
+      <c r="B10">
+        <v>3019</v>
+      </c>
+      <c r="C10">
+        <v>699</v>
+      </c>
+      <c r="D10">
+        <v>2669</v>
+      </c>
+      <c r="E10">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>3049</v>
+      </c>
+      <c r="B11">
+        <v>3019</v>
+      </c>
+      <c r="C11">
+        <v>719</v>
+      </c>
+      <c r="D11">
+        <v>719</v>
+      </c>
+      <c r="E11">
+        <v>2669</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="3"/>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="3"/>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="3"/>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="3"/>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="3"/>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="3"/>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="3"/>
+    </row>
+  </sheetData>
+  <dataConsolidate function="count"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2466C675-5B49-4BE3-A3BD-B98A43213ECB}">
+  <dimension ref="A1:A51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>2669</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4">
+        <v>3048</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7">
+        <v>3048</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <v>2669</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11">
+        <v>3049</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12">
+        <v>2669</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15">
+        <v>3019</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16">
+        <v>2669</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19">
+        <v>3049</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20">
+        <v>3019</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21">
+        <v>3019</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22">
+        <v>2669</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24">
+        <v>2669</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25">
+        <v>2669</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26">
+        <v>3019</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27">
+        <v>2668</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29">
+        <v>2669</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33">
+        <v>3019</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37">
+        <v>3019</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39">
+        <v>3019</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40">
+        <v>2669</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47">
+        <v>3018</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48">
+        <v>3019</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51">
+        <v>2669</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>